<commit_message>
Add CYRS Review Sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -159,49 +159,12 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The CYRS describe the overall system and shall be more abstracted from the level of SW. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You need to make your requirement more clarified from the system level prospective. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Req_ PO2_EBL_Electric_Blender_CYRS_001-1.0: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- There’s no need to mention the first speed with duty cycle and instead of that you could say for example : 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">the blender shall operate between 3 different speeds (Speed1 → Speed 2 → Speed 3) triggered by a button.
+      <t xml:space="preserve">The CYRS describe the overall system and shall be more abstracted from the level of SW. You need to make your requirement more clarified from the system level prospective. 
+Req_ PO2_EBL_Electric_Blender_CYRS_001-1.0: 
+- There’s no need to mention the first speed with duty cycle and instead of that you could say for example : 
+the blender shall operate between 3 different speeds (Speed1 → Speed 2 → Speed 3) triggered by a button.
 - Also, t</t>
     </r>
     <r>
@@ -210,6 +173,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">here isn’t a customer specification states that the first speed with duty cycle of 50%. You shouldn’t take a step forward and guess something not mentioned by the customer in CRS until taking customer approval. </t>
     </r>
@@ -245,7 +209,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -292,16 +256,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -486,7 +445,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -579,26 +538,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -619,7 +562,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -627,7 +570,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -783,7 +726,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -1028,7 +971,7 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
@@ -1101,16 +1044,16 @@
       <c r="B3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="21" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="22"/>
@@ -1154,7 +1097,7 @@
       <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="18" t="s">
@@ -1163,7 +1106,7 @@
       <c r="E5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="23" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="22"/>
@@ -1182,7 +1125,7 @@
       <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -1191,7 +1134,7 @@
       <c r="E6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="22"/>
@@ -1207,7 +1150,7 @@
       <c r="B7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -1216,7 +1159,7 @@
       <c r="E7" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="23" t="s">
         <v>43</v>
       </c>
       <c r="G7" s="22"/>
@@ -1228,7 +1171,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="23"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="18"/>
       <c r="E8" s="20"/>
       <c r="F8" s="21"/>
@@ -1242,7 +1185,7 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
-      <c r="C9" s="23"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="18"/>
       <c r="E9" s="20"/>
       <c r="F9" s="21"/>
@@ -1343,356 +1286,356 @@
       <c r="I16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="33"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="33"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="32"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="33"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="33"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="33"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="33"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="33"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="33"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
-      <c r="I25" s="33"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
-      <c r="I26" s="33"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
-      <c r="I27" s="33"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
-      <c r="I28" s="33"/>
+      <c r="I28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="35"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
-      <c r="I29" s="33"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="35"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="33"/>
+      <c r="I30" s="29"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="33"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="36"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
-      <c r="I32" s="33"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="35"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="33"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="35"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
-      <c r="I34" s="33"/>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="33"/>
+      <c r="I35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="35"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="33"/>
+      <c r="I36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="35"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="33"/>
+      <c r="I37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="35"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="33"/>
+      <c r="I38" s="29"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="35"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="31"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="33"/>
+      <c r="I39" s="29"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="35"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="31"/>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
-      <c r="I40" s="33"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="35"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-      <c r="I41" s="33"/>
+      <c r="I41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="35"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="31"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
-      <c r="I42" s="33"/>
+      <c r="I42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="35"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="31"/>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
-      <c r="I43" s="33"/>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="35"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="31"/>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
-      <c r="I44" s="33"/>
+      <c r="I44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="35"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="31"/>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
-      <c r="I45" s="33"/>
+      <c r="I45" s="29"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="35"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="31"/>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
-      <c r="I46" s="33"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="35"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="31"/>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
-      <c r="I47" s="33"/>
+      <c r="I47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="35"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="31"/>
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
-      <c r="I48" s="33"/>
+      <c r="I48" s="29"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">

</xml_diff>

<commit_message>
Accepting the Review Points in the CYRS & HSI Review Sheets
Assigning tasks to the team mates and adding them in the project plan

Signed-off-by: mostafamoh1236 <mostafamoh1236@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction " sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction " sheetId="1" r:id="rId1"/>
+    <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">'Cross review points '!$F$8</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">'Cross review points '!$F$8</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -41,28 +40,28 @@
     <t xml:space="preserve">Ref Version </t>
   </si>
   <si>
-    <t xml:space="preserve">V1.2</t>
+    <t>V1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Auther </t>
   </si>
   <si>
-    <t xml:space="preserve">Tarek Sharaby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auther</t>
+    <t>Tarek Sharaby</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>24/01/2020</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Auther</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -71,83 +70,83 @@
     <t xml:space="preserve">Change </t>
   </si>
   <si>
-    <t xml:space="preserve">T.Sharaby</t>
+    <t>T.Sharaby</t>
   </si>
   <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Entry Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page/Line/Section/Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open point : description of problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neither the Status nor the version and the project ID has been written in the first page of CYRS document , you could add a header table appears in each page of the document.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 3</t>
+    <t>Entry Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Detection version</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>Page/Line/Section/Entity</t>
+  </si>
+  <si>
+    <t>Open point : description of problem</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>29/01/2020</t>
+  </si>
+  <si>
+    <t>A.Ali</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>Page 1</t>
+  </si>
+  <si>
+    <t>Neither the Status nor the version and the project ID has been written in the first page of CYRS document , you could add a header table appears in each page of the document.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Page 3</t>
   </si>
   <si>
     <t xml:space="preserve">
 - Document history has to be at the start before Table of Contents. </t>
   </si>
   <si>
-    <t xml:space="preserve">Table of Contents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Table of Content page numbering for all sections.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last page</t>
+    <t>Table of Contents</t>
+  </si>
+  <si>
+    <t>Update Table of Content page numbering for all sections.</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Last page</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even CYRS should have one and the reference is the customer Requirement for the product </t>
   </si>
   <si>
-    <t xml:space="preserve">Refused</t>
+    <t>Refused</t>
   </si>
   <si>
     <t xml:space="preserve">Features </t>
@@ -161,7 +160,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The CYRS describe the overall system and shall be more abstracted from the level of SW. You need to make your requirement more clarified from the system level prospective. 
+      <t>The CYRS describe the overall system and shall be more abstracted from the level of SW. You need to make your requirement more clarified from the system level prospective. 
 Req_ PO2_EBL_Electric_Blender_CYRS_001-1.0: 
 - There’s no need to mention the first speed with duty cycle and instead of that you could say for example : 
 the blender shall operate between 3 different speeds (Speed1 → Speed 2 → Speed 3) triggered by a button.
@@ -179,11 +178,11 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">All Req need to be updated with system level prospective not SW prospective. 
+    <t>All Req need to be updated with system level prospective not SW prospective. 
 (Req_ PO2_EBL_Electric_Blender_CYRS_002-1.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">Resolved</t>
+    <t>Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Decision </t>
@@ -202,14 +201,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]General"/>
-    <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]General"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -218,22 +215,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -241,7 +223,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -264,6 +246,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -297,103 +286,149 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -409,203 +444,151 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 3 2" xfId="20"/>
-    <cellStyle name="Normal 4" xfId="21"/>
-    <cellStyle name="Excel Built-in Accent3" xfId="22"/>
+    <cellStyle name="Normal 3 2" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF808080"/>
+        <color rgb="FFFBE5D6"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF535353"/>
       </font>
@@ -617,41 +600,18 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF385724"/>
+        <color rgb="FF808080"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -710,223 +670,514 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:H18"/>
+  <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:8">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="n">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="12">
         <v>0.1</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="12"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="12"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="12"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="12"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="13"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -934,56 +1185,44 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" customWidth="1"/>
+    <col min="8" max="9" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1031,13 +1270,15 @@
       <c r="F2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="H2" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -1056,13 +1297,15 @@
       <c r="F3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="H3" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I3" s="22"/>
     </row>
-    <row r="4" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="20.45" customHeight="1">
       <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
@@ -1081,16 +1324,18 @@
       <c r="F4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="H4" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I4" s="22"/>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
@@ -1109,16 +1354,18 @@
       <c r="F5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="H5" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I5" s="22"/>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="82.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" ht="122.25">
       <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
@@ -1137,13 +1384,15 @@
       <c r="F6" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="22"/>
+      <c r="G6" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="H6" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" ht="52.15" customHeight="1">
       <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
@@ -1162,13 +1411,15 @@
       <c r="F7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="H7" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
@@ -1178,11 +1429,11 @@
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="20"/>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -1192,11 +1443,11 @@
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="20"/>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -1207,7 +1458,7 @@
       <c r="H10" s="22"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1218,7 +1469,7 @@
       <c r="H11" s="22"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1228,14 +1479,14 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="20"/>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="L12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1245,14 +1496,14 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="20"/>
-      <c r="K13" s="0" t="s">
+      <c r="K13" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="0" t="s">
+      <c r="L13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1263,7 +1514,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1274,7 +1525,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -1285,7 +1536,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -1296,7 +1547,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9">
       <c r="A18" s="24"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -1307,7 +1558,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9">
       <c r="A19" s="24"/>
       <c r="B19" s="25"/>
       <c r="C19" s="26"/>
@@ -1318,7 +1569,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -1329,7 +1580,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9">
       <c r="A21" s="24"/>
       <c r="B21" s="25"/>
       <c r="C21" s="26"/>
@@ -1340,7 +1591,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
@@ -1351,7 +1602,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
@@ -1362,7 +1613,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9">
       <c r="A24" s="24"/>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
@@ -1373,7 +1624,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9">
       <c r="A25" s="24"/>
       <c r="B25" s="25"/>
       <c r="C25" s="26"/>
@@ -1384,7 +1635,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9">
       <c r="A26" s="24"/>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
@@ -1395,7 +1646,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9">
       <c r="A27" s="24"/>
       <c r="B27" s="25"/>
       <c r="C27" s="26"/>
@@ -1406,7 +1657,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9">
       <c r="A28" s="24"/>
       <c r="B28" s="25"/>
       <c r="C28" s="26"/>
@@ -1417,7 +1668,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
@@ -1428,7 +1679,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9">
       <c r="A30" s="24"/>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -1439,7 +1690,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="29"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9">
       <c r="A31" s="24"/>
       <c r="B31" s="25"/>
       <c r="C31" s="25"/>
@@ -1450,7 +1701,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="29"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9">
       <c r="A32" s="24"/>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
@@ -1461,7 +1712,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="29"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -1472,7 +1723,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="29"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9">
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -1483,7 +1734,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="29"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9">
       <c r="A35" s="24"/>
       <c r="B35" s="25"/>
       <c r="C35" s="25"/>
@@ -1494,7 +1745,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="29"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9">
       <c r="A36" s="26"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
@@ -1505,7 +1756,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="29"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:9">
       <c r="A37" s="26"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
@@ -1516,7 +1767,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="29"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:9">
       <c r="A38" s="26"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
@@ -1527,7 +1778,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="29"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:9">
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
@@ -1538,7 +1789,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="29"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:9">
       <c r="A40" s="26"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
@@ -1549,7 +1800,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="29"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9">
       <c r="A41" s="26"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
@@ -1560,7 +1811,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="29"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:9">
       <c r="A42" s="26"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
@@ -1571,7 +1822,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="29"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:9">
       <c r="A43" s="26"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
@@ -1582,7 +1833,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="29"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:9">
       <c r="A44" s="26"/>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
@@ -1593,7 +1844,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="29"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:9">
       <c r="A45" s="26"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
@@ -1604,7 +1855,7 @@
       <c r="H45" s="22"/>
       <c r="I45" s="29"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:9">
       <c r="A46" s="26"/>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
@@ -1615,7 +1866,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="29"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:9">
       <c r="A47" s="26"/>
       <c r="B47" s="26"/>
       <c r="C47" s="26"/>
@@ -1626,7 +1877,7 @@
       <c r="H47" s="22"/>
       <c r="I47" s="29"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:9">
       <c r="A48" s="26"/>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
@@ -1639,40 +1890,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1048" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1048" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048">
       <formula1>$K$8:$K$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changing back the status of the reviews in CYRS & HSI to Open as i didn't notice that it should be changed by the reviewer
Signed-off-by: mostafamoh1236 <mostafamoh1236@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -452,36 +452,6 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -541,6 +511,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -980,189 +980,213 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="28"/>
+      <c r="G12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="12">
+      <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="12"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="12"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="12"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="12"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="13"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1172,30 +1196,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1223,262 +1223,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="34.15" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="22"/>
+      <c r="H2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:12" ht="30">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="22"/>
+      <c r="H3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:12" ht="20.45" customHeight="1">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="22"/>
+      <c r="H4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="12"/>
       <c r="K4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="22"/>
+      <c r="H5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="12"/>
       <c r="K5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="122.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="22"/>
+      <c r="H6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:12" ht="52.15" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="20"/>
+      <c r="H7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="20"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="10"/>
       <c r="K8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="20"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="10"/>
       <c r="K9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="20"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="20"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="20"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="10"/>
       <c r="K12" t="s">
         <v>45</v>
       </c>
@@ -1487,15 +1487,15 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="10"/>
       <c r="K13" t="s">
         <v>47</v>
       </c>
@@ -1504,389 +1504,389 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="20"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="20"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="20"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="29"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="29"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="29"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="29"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="29"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="29"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="29"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="29"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="29"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="29"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="29"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="29"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="29"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="29"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="29"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="29"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="29"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="29"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="24"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="29"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="19"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="29"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="19"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="29"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="29"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="19"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="29"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="19"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="29"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="19"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="29"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="29"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="29"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="29"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="19"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="29"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="19"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="29"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="29"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="19"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="29"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">

</xml_diff>

<commit_message>
- Accepting the review points in the CYRS_review sheet - Accepting the review points in the HSI_review sheet - Accepting the review points in the SRS_review sheet - updating the Project plan document with the new tasks, estimated deadlines and who is assigned to each task
Signed-off-by: mostafamoh1236 <mostafamoh1236@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction " sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction " sheetId="1" r:id="rId1"/>
+    <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">'Cross review points '!$F$8</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">'Cross review points '!$F$8</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
   <si>
-    <t xml:space="preserve">Electric Blender</t>
+    <t>Electric Blender</t>
   </si>
   <si>
     <t xml:space="preserve">Ref Document </t>
@@ -41,25 +40,25 @@
     <t xml:space="preserve">Ref Version </t>
   </si>
   <si>
-    <t xml:space="preserve">V1.1</t>
+    <t>V1.1</t>
   </si>
   <si>
     <t xml:space="preserve">Auther </t>
   </si>
   <si>
-    <t xml:space="preserve">Abdelrahman Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auther</t>
+    <t>Abdelrahman Ali</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Auther</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -68,86 +67,86 @@
     <t xml:space="preserve">Change </t>
   </si>
   <si>
-    <t xml:space="preserve">A.Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/01/2020</t>
+    <t>A.Ali</t>
+  </si>
+  <si>
+    <t>31/01/2020</t>
   </si>
   <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Close old points from week 1 &amp; Add new points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entry Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page/Line/Section/Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open point : description of problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neither the Status nor the version and the project ID has been written in the first page of CYRS document , you could add a header table appears in each page of the document.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 3</t>
+    <t>Close old points from week 1 &amp; Add new points</t>
+  </si>
+  <si>
+    <t>Entry Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Detection version</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>Page/Line/Section/Entity</t>
+  </si>
+  <si>
+    <t>Open point : description of problem</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>29/01/2020</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>Page 1</t>
+  </si>
+  <si>
+    <t>Neither the Status nor the version and the project ID has been written in the first page of CYRS document , you could add a header table appears in each page of the document.</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Page 3</t>
   </si>
   <si>
     <t xml:space="preserve">
 Document history has to be at the start before Table of Contents. </t>
   </si>
   <si>
-    <t xml:space="preserve">Table of Contents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Table of Content page numbering for all sections.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last page</t>
+    <t>Table of Contents</t>
+  </si>
+  <si>
+    <t>Update Table of Content page numbering for all sections.</t>
+  </si>
+  <si>
+    <t>Last page</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even CYRS should have one and the reference is the customer Requirement for the product </t>
   </si>
   <si>
-    <t xml:space="preserve">Refused</t>
+    <t>Refused</t>
   </si>
   <si>
     <t xml:space="preserve">Features </t>
@@ -161,7 +160,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The CYRS describe the overall system and shall be more abstracted from the level of SW. You need to make your requirement more clarified from the system level prospective. 
+      <t>The CYRS describe the overall system and shall be more abstracted from the level of SW. You need to make your requirement more clarified from the system level prospective. 
 Req_ PO2_EBL_Electric_Blender_CYRS_001-1.0: 
 - There’s no need to mention the first speed with duty cycle and instead of that you could say for example : 
 the blender shall operate between 3 different speeds (Speed1 → Speed 2 → Speed 3) triggered by a button.
@@ -179,30 +178,30 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">All Req need to be updated with system level prospective not SW prospective. 
+    <t>All Req need to be updated with system level prospective not SW prospective. 
 (Req_ PO2_EBL_Electric_Blender_CYRS_002-1.0)</t>
   </si>
   <si>
     <t xml:space="preserve">Reference Table </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference table title should be before the table not after it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
+    <t>Reference table title should be before the table not after it.</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
   <si>
     <t xml:space="preserve">Can’t navigate to table of figures page numbering from Table of Contents. </t>
   </si>
   <si>
-    <t xml:space="preserve">Document History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add separate date for rework &amp; review in Document History table even if the work is done in the same day. 
+    <t>Document History</t>
+  </si>
+  <si>
+    <t>Add separate date for rework &amp; review in Document History table even if the work is done in the same day. 
 According to the plan, CYRS review planned to start on 5/2/2020.</t>
   </si>
   <si>
-    <t xml:space="preserve">System Requirements</t>
+    <t>System Requirements</t>
   </si>
   <si>
     <r>
@@ -224,7 +223,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Req_ PO2_EBL_Electric_Blender_CYRS_003-1.0</t>
+      <t>Req_ PO2_EBL_Electric_Blender_CYRS_003-1.0</t>
     </r>
   </si>
   <si>
@@ -237,7 +236,7 @@
     <t xml:space="preserve">whether to accept the open point if you see applicable and valid or to refuse it and give a justification in the comment field whether you accept , then update with the action you did , or refuse with justification </t>
   </si>
   <si>
-    <t xml:space="preserve">You need to add more requirements in CYRS. 
+    <t>You need to add more requirements in CYRS. 
 Ex: you can  add requirements which describe how to handle the communication between the inputs devices &amp; o/p devices (Motor driver &amp; Motor).</t>
   </si>
   <si>
@@ -245,22 +244,26 @@
   </si>
   <si>
     <t xml:space="preserve">Is for the reviewer he check the fix of the open point and check if the fix is ok or still open </t>
+  </si>
+  <si>
+    <t>Reference table title is already before the table not after it</t>
+  </si>
+  <si>
+    <t>the table of figures is in the same page of table of content, could you clarify your point more ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]General"/>
-    <numFmt numFmtId="168" formatCode="[$-409]M/D/YYYY"/>
-    <numFmt numFmtId="169" formatCode="@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]MM/DD/YY"/>
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]General"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
+    <numFmt numFmtId="168" formatCode="[$-409]mm/dd/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -269,22 +272,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -298,7 +286,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -321,6 +309,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -354,103 +349,149 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -466,215 +507,160 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 3 2" xfId="20"/>
-    <cellStyle name="Normal 4" xfId="21"/>
-    <cellStyle name="Excel Built-in Accent3" xfId="22"/>
+    <cellStyle name="Normal 3 2" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF808080"/>
+        <color rgb="FFFBE5D6"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF535353"/>
       </font>
@@ -686,41 +672,18 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF385724"/>
+        <color rgb="FF808080"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -779,230 +742,522 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:8">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4" t="n">
+      <c r="C9" s="12"/>
+      <c r="D9" s="9">
         <v>44014</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="14">
         <v>0.1</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="n">
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="14">
         <v>0.2</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12" t="n">
+      <c r="D14" s="4"/>
+      <c r="E14" s="3">
         <v>44014</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="14"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="14"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="14"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="15"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -1010,56 +1265,45 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
@@ -1088,7 +1332,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
@@ -1115,7 +1359,7 @@
       </c>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
@@ -1142,7 +1386,7 @@
       </c>
       <c r="I3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="20.45" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -1168,11 +1412,11 @@
         <v>33</v>
       </c>
       <c r="I4" s="24"/>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
@@ -1198,11 +1442,11 @@
         <v>33</v>
       </c>
       <c r="I5" s="24"/>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="94.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" ht="122.25">
       <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
@@ -1229,7 +1473,7 @@
       </c>
       <c r="I6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
@@ -1256,8 +1500,8 @@
       </c>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="n">
+    <row r="8" spans="1:12" ht="102" customHeight="1">
+      <c r="A8" s="26">
         <v>44014</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -1275,17 +1519,21 @@
       <c r="F8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="H8" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="K8" s="0" t="s">
+      <c r="I8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="n">
+    <row r="9" spans="1:12" ht="66" customHeight="1">
+      <c r="A9" s="26">
         <v>44014</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1303,17 +1551,21 @@
       <c r="F9" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="H9" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="K9" s="0" t="s">
+      <c r="I9" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26" t="n">
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" s="26">
         <v>44014</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -1331,14 +1583,16 @@
       <c r="F10" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="H10" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="n">
+    <row r="11" spans="1:12" ht="60">
+      <c r="A11" s="26">
         <v>44014</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -1356,14 +1610,16 @@
       <c r="F11" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="n">
+    <row r="12" spans="1:12" ht="48" customHeight="1">
+      <c r="A12" s="26">
         <v>44014</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -1381,20 +1637,22 @@
       <c r="F12" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I12" s="22"/>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="L12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="n">
+    <row r="13" spans="1:12" ht="45">
+      <c r="A13" s="26">
         <v>44014</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -1412,19 +1670,21 @@
       <c r="F13" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="H13" s="24" t="s">
         <v>46</v>
       </c>
       <c r="I13" s="22"/>
-      <c r="K13" s="0" t="s">
+      <c r="K13" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="0" t="s">
+      <c r="L13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12">
       <c r="A14" s="26"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -1435,7 +1695,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
@@ -1446,7 +1706,7 @@
       <c r="H15" s="24"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
@@ -1457,7 +1717,7 @@
       <c r="H16" s="24"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -1468,7 +1728,7 @@
       <c r="H17" s="24"/>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9">
       <c r="A18" s="27"/>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -1479,7 +1739,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="32"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9">
       <c r="A19" s="27"/>
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
@@ -1490,7 +1750,7 @@
       <c r="H19" s="24"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9">
       <c r="A20" s="27"/>
       <c r="B20" s="28"/>
       <c r="C20" s="29"/>
@@ -1501,7 +1761,7 @@
       <c r="H20" s="24"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9">
       <c r="A21" s="27"/>
       <c r="B21" s="28"/>
       <c r="C21" s="29"/>
@@ -1512,7 +1772,7 @@
       <c r="H21" s="24"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9">
       <c r="A22" s="27"/>
       <c r="B22" s="28"/>
       <c r="C22" s="29"/>
@@ -1523,7 +1783,7 @@
       <c r="H22" s="24"/>
       <c r="I22" s="32"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9">
       <c r="A23" s="27"/>
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
@@ -1534,7 +1794,7 @@
       <c r="H23" s="24"/>
       <c r="I23" s="32"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9">
       <c r="A24" s="27"/>
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
@@ -1545,7 +1805,7 @@
       <c r="H24" s="24"/>
       <c r="I24" s="32"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9">
       <c r="A25" s="27"/>
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
@@ -1556,7 +1816,7 @@
       <c r="H25" s="24"/>
       <c r="I25" s="32"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9">
       <c r="A26" s="27"/>
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
@@ -1567,7 +1827,7 @@
       <c r="H26" s="24"/>
       <c r="I26" s="32"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9">
       <c r="A27" s="27"/>
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
@@ -1578,7 +1838,7 @@
       <c r="H27" s="24"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9">
       <c r="A28" s="27"/>
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
@@ -1589,7 +1849,7 @@
       <c r="H28" s="24"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9">
       <c r="A29" s="29"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -1600,7 +1860,7 @@
       <c r="H29" s="24"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9">
       <c r="A30" s="27"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -1611,7 +1871,7 @@
       <c r="H30" s="24"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9">
       <c r="A31" s="27"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -1622,7 +1882,7 @@
       <c r="H31" s="24"/>
       <c r="I31" s="32"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9">
       <c r="A32" s="27"/>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
@@ -1633,7 +1893,7 @@
       <c r="H32" s="24"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9">
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -1644,7 +1904,7 @@
       <c r="H33" s="24"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
@@ -1655,7 +1915,7 @@
       <c r="H34" s="24"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9">
       <c r="A35" s="27"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
@@ -1666,7 +1926,7 @@
       <c r="H35" s="24"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9">
       <c r="A36" s="29"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
@@ -1677,7 +1937,7 @@
       <c r="H36" s="24"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:9">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -1688,7 +1948,7 @@
       <c r="H37" s="24"/>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:9">
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
@@ -1699,7 +1959,7 @@
       <c r="H38" s="24"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:9">
       <c r="A39" s="29"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
@@ -1710,7 +1970,7 @@
       <c r="H39" s="24"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:9">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -1721,7 +1981,7 @@
       <c r="H40" s="24"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9">
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
@@ -1732,7 +1992,7 @@
       <c r="H41" s="24"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:9">
       <c r="A42" s="29"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -1743,7 +2003,7 @@
       <c r="H42" s="24"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:9">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -1754,7 +2014,7 @@
       <c r="H43" s="24"/>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:9">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
@@ -1765,7 +2025,7 @@
       <c r="H44" s="24"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:9">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
@@ -1776,7 +2036,7 @@
       <c r="H45" s="24"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:9">
       <c r="A46" s="29"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
@@ -1787,7 +2047,7 @@
       <c r="H46" s="24"/>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:9">
       <c r="A47" s="29"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
@@ -1798,7 +2058,7 @@
       <c r="H47" s="24"/>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:9">
       <c r="A48" s="29"/>
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>
@@ -1811,40 +2071,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1048" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1048" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048">
       <formula1>$K$8:$K$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify CYRS document version 1.3 after the Review on version 1.2 concerning the following: 1-Modify the 2nd & 3rd requirements and its version 2-adding 4th requirement Signed-off-by: madel-anis <madel.anis11@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Software Engineering\Electric_Blender\Input documents\CYRS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22C1EFB-B989-40CA-8A83-F915BD8F96D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -255,7 +261,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
@@ -263,7 +269,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
     <numFmt numFmtId="168" formatCode="[$-409]mm/dd/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -515,42 +521,6 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -614,12 +584,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
+    <cellStyle name="Excel Built-in Accent3" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -752,6 +758,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -798,7 +812,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -830,9 +844,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,6 +896,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1039,210 +1089,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="12" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="12" t="s">
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="12" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="12" t="s">
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="9">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33">
         <v>44014</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="7" t="s">
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="13" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5" t="s">
+      <c r="F12" s="30"/>
+      <c r="G12" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="14">
+      <c r="H12" s="31"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="26"/>
+      <c r="E13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="10" t="s">
+      <c r="F13" s="26"/>
+      <c r="G13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="14">
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
         <v>0.2</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3">
+      <c r="D14" s="26"/>
+      <c r="E14" s="28">
         <v>44014</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="10" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="14"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" s="14"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="14"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="15"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1252,30 +1326,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1283,14 +1333,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -1298,352 +1348,353 @@
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="100.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="30.5703125" customWidth="1"/>
     <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.15" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="24"/>
-    </row>
-    <row r="3" spans="1:12" ht="30">
-      <c r="A3" s="19" t="s">
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="24"/>
-    </row>
-    <row r="4" spans="1:12" ht="20.45" customHeight="1">
-      <c r="A4" s="19" t="s">
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="24"/>
+      <c r="I4" s="12"/>
       <c r="K4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="12"/>
       <c r="K5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="122.25">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:12" ht="122.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" s="19" t="s">
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="22"/>
-    </row>
-    <row r="8" spans="1:12" ht="102" customHeight="1">
-      <c r="A8" s="26">
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>44014</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="10" t="s">
         <v>58</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="66" customHeight="1">
-      <c r="A9" s="26">
+    <row r="9" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
         <v>44014</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="10" t="s">
         <v>59</v>
       </c>
       <c r="K9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="26">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
         <v>44014</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" spans="1:12" ht="60">
-      <c r="A11" s="26">
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
         <v>44014</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:12" ht="48" customHeight="1">
-      <c r="A12" s="26">
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
         <v>44014</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="22"/>
+      <c r="I12" s="10"/>
       <c r="K12" t="s">
         <v>53</v>
       </c>
@@ -1651,32 +1702,32 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45">
-      <c r="A13" s="26">
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <v>44014</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="22"/>
+      <c r="I13" s="10"/>
       <c r="K13" t="s">
         <v>56</v>
       </c>
@@ -1684,390 +1735,390 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="26"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="32"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="32"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="32"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="32"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="32"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="32"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="32"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="32"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="32"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="32"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="32"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="32"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="32"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="32"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="32"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="32"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="32"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="32"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="32"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="32"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="32"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="32"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="32"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="32"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="32"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="32"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="32"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="32"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="32"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="32"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="20"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="20"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="20"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="20"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="20"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
@@ -2090,11 +2141,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$8:$K$9</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>